<commit_message>
Adding the new search results
</commit_message>
<xml_diff>
--- a/combined_lethal_phenotypes.xlsx
+++ b/combined_lethal_phenotypes.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$1529</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -56275,7 +56275,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1">
+  <autoFilter ref="A1:J1529">
     <sortState ref="A2:J1529">
       <sortCondition ref="A1:A1529"/>
     </sortState>

</xml_diff>